<commit_message>
v 1.0.13 version prod
</commit_message>
<xml_diff>
--- a/Data/Parameters/Parámetros Revisión de Asientos Manuales de Compensación.xlsx
+++ b/Data/Parameters/Parámetros Revisión de Asientos Manuales de Compensación.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S_RPA_CORP\Downloads\VOTORANTIM_001_RT1_SOX-rfernandez\VOTORANTIM_001_RT1_SOX-rfernandez\Data\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S_RPA_CORP\Documents\UiPath\VOTOR-SOX-2024-002 Controles SOX-EAA-01.74.1-AR y SOX-EAA-02.74.1-AP y GL\Data\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DADEE5-F099-4F7E-AC48-6879BCE6550B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC57A891-28E0-44AB-8731-D47210BCEFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="9705" xr2:uid="{D9BD6469-DA06-4086-A45A-FED19CB1C737}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D9BD6469-DA06-4086-A45A-FED19CB1C737}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="2" r:id="rId1"/>
@@ -158,7 +158,7 @@
     <t>E002, E009, E026, E033, E061</t>
   </si>
   <si>
-    <t>lucy.serrano@vcimentos.com;javier.martin@vcimentos.com</t>
+    <t>lucy.serrano@vcimentos.com;javier.martin@vcimentos.com;sat@rpatechnologies.es</t>
   </si>
 </sst>
 </file>
@@ -217,7 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -249,7 +249,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3675D7FC-4954-4306-83A3-4337972F2C8C}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J2:L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,13 +731,13 @@
       <c r="I2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" t="s">
         <v>40</v>
       </c>
       <c r="M2" s="6" t="s">
@@ -779,13 +778,13 @@
       <c r="I3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" t="s">
         <v>40</v>
       </c>
       <c r="M3" s="6" t="s">
@@ -826,13 +825,13 @@
       <c r="I4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="6" t="s">

</xml_diff>